<commit_message>
feat: Added province field
</commit_message>
<xml_diff>
--- a/tests/excel_para_teste.xlsx
+++ b/tests/excel_para_teste.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>EMAIL</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t xml:space="preserve">CLASSROOMS </t>
+  </si>
+  <si>
+    <t>PROVINCE</t>
+  </si>
+  <si>
+    <t>{"nome":"Luanda","id": 1}</t>
   </si>
 </sst>
 </file>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -390,9 +396,10 @@
     <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -402,8 +409,11 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -413,8 +423,11 @@
       <c r="C2">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -424,8 +437,11 @@
       <c r="C3">
         <v>7</v>
       </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -434,6 +450,9 @@
       </c>
       <c r="C4">
         <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Fixed usage of province
</commit_message>
<xml_diff>
--- a/tests/excel_para_teste.xlsx
+++ b/tests/excel_para_teste.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>EMAIL</t>
   </si>
@@ -53,10 +53,7 @@
     <t xml:space="preserve">CLASSROOMS </t>
   </si>
   <si>
-    <t>PROVINCE</t>
-  </si>
-  <si>
-    <t>{"nome":"Luanda","id": 1}</t>
+    <t>ID_PROVINCE</t>
   </si>
 </sst>
 </file>
@@ -388,7 +385,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -423,8 +420,8 @@
       <c r="C2">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
+      <c r="D2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -437,8 +434,8 @@
       <c r="C3">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
+      <c r="D3">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -451,8 +448,8 @@
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
+      <c r="D4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Altered test domain
</commit_message>
<xml_diff>
--- a/tests/excel_para_teste.xlsx
+++ b/tests/excel_para_teste.xlsx
@@ -435,7 +435,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -449,7 +449,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>